<commit_message>
changes in results tree
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS_SAND/Data/Assortment.xlsx
+++ b/Projects/DIAGEOUS_SAND/Data/Assortment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Granular Groups" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="24">
   <si>
     <t>Granular Group Name</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>Store_Att_1 Value</t>
+  </si>
+  <si>
+    <t>Store_Att_2 Name</t>
+  </si>
+  <si>
+    <t>Store_Att_2 Value</t>
+  </si>
+  <si>
+    <t>Store_Att_3 Name</t>
+  </si>
+  <si>
+    <t>Store_Att_3 Value</t>
+  </si>
+  <si>
+    <t>Store_Att_4 Name</t>
+  </si>
+  <si>
+    <t>Store_Att_4 Value</t>
+  </si>
+  <si>
+    <t>Store_Att_5 Name</t>
+  </si>
+  <si>
+    <t>Store_Att_5 Value</t>
   </si>
   <si>
     <t>store_id</t>
@@ -326,15 +350,15 @@
   </sheetPr>
   <dimension ref="A1:E224"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C222" activeCellId="0" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="4" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="4" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
@@ -4138,21 +4162,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C65536"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="96.6194331983806"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.4777327935223"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3238866396761"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.96761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4162,13 +4189,37 @@
       <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -4179,7 +4230,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>8</v>
@@ -4190,7 +4241,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>9</v>
@@ -4250,7 +4301,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
@@ -4261,7 +4312,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -4270,7 +4321,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>